<commit_message>
Update summary results with the Korea numbers
</commit_message>
<xml_diff>
--- a/summary_data/gftpF_summary.xlsx
+++ b/summary_data/gftpF_summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isfiligoi/github/tnrp-net-tests/summary_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B2CB364-1CCD-744A-852F-F407C84BD9E6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{730E258B-36D8-3141-8455-F3DD9BC06CC0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="-21900" windowWidth="22920" windowHeight="17440" xr2:uid="{F871B44F-434F-FB4B-AC1F-99327B90C475}"/>
+    <workbookView xWindow="840" yWindow="-25400" windowWidth="22920" windowHeight="17440" xr2:uid="{F871B44F-434F-FB4B-AC1F-99327B90C475}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>Server</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>GridFTP tests - fast with callback</t>
+  </si>
+  <si>
+    <t>Korea</t>
   </si>
 </sst>
 </file>
@@ -441,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3AE2A42-D91B-564A-AB68-339151ECBD6D}">
-  <dimension ref="A1:N22"/>
+  <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -452,22 +455,22 @@
     <col min="11" max="11" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -502,13 +505,16 @@
         <v>7</v>
       </c>
       <c r="M5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="O5" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>2</v>
       </c>
@@ -528,14 +534,15 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
-      <c r="M6" s="1">
+      <c r="M6" s="1"/>
+      <c r="N6" s="1">
         <v>27.4</v>
       </c>
-      <c r="N6" s="1">
+      <c r="O6" s="1">
         <v>27.1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>3</v>
       </c>
@@ -559,10 +566,13 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
+      <c r="M7" s="1">
+        <v>19.100000000000001</v>
+      </c>
       <c r="N7" s="1"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O7" s="1"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>13</v>
       </c>
@@ -590,8 +600,11 @@
       <c r="L8">
         <v>11.9</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M8">
+        <v>14.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>8</v>
       </c>
@@ -604,14 +617,14 @@
       <c r="F9">
         <v>7.1</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>20.5</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <v>21.5</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>6</v>
       </c>
@@ -640,13 +653,16 @@
         <v>10.8</v>
       </c>
       <c r="M10">
+        <v>14.3</v>
+      </c>
+      <c r="N10">
         <v>18.8</v>
       </c>
-      <c r="N10">
+      <c r="O10">
         <v>43.5</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>7</v>
       </c>
@@ -662,31 +678,31 @@
       <c r="L11">
         <v>7.4</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>20</v>
       </c>
-      <c r="N11">
+      <c r="O11">
         <v>21.7</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B15" t="str">
         <f>B4</f>
         <v>Server</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="str">
         <f>A5</f>
         <v>Client</v>
       </c>
       <c r="C16" t="str">
-        <f t="shared" ref="C16:N16" si="0">C5</f>
+        <f t="shared" ref="C16:O16" si="0">C5</f>
         <v>AWS EU W1</v>
       </c>
       <c r="D16" t="str">
@@ -727,14 +743,18 @@
       </c>
       <c r="M16" t="str">
         <f t="shared" si="0"/>
+        <v>Korea</v>
+      </c>
+      <c r="N16" t="str">
+        <f t="shared" si="0"/>
         <v>AWS Korea</v>
       </c>
-      <c r="N16" t="str">
+      <c r="O16" t="str">
         <f t="shared" si="0"/>
         <v>AWS Australia</v>
       </c>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B17" t="str">
         <f>B6</f>
         <v>AWS EU C1</v>
@@ -751,22 +771,22 @@
         <f>100/F6</f>
         <v>5.1020408163265305</v>
       </c>
-      <c r="M17" s="2">
-        <f>100/M6</f>
-        <v>3.6496350364963503</v>
-      </c>
       <c r="N17" s="2">
         <f>100/N6</f>
+        <v>3.6496350364963503</v>
+      </c>
+      <c r="O17" s="2">
+        <f>100/O6</f>
         <v>3.6900369003690034</v>
       </c>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B18" t="str">
         <f t="shared" ref="B18:B22" si="2">B7</f>
         <v>Amsterdam</v>
       </c>
       <c r="C18" s="2">
-        <f t="shared" ref="C18:L21" si="3">100/C7</f>
+        <f t="shared" ref="C18:M21" si="3">100/C7</f>
         <v>9.1743119266055047</v>
       </c>
       <c r="D18" s="2">
@@ -785,10 +805,14 @@
         <f t="shared" ref="I18" si="4">100/I7</f>
         <v>7.9365079365079367</v>
       </c>
-      <c r="M18" s="2"/>
+      <c r="M18" s="2">
+        <f t="shared" si="3"/>
+        <v>5.2356020942408374</v>
+      </c>
       <c r="N18" s="2"/>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O18" s="2"/>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B19" t="str">
         <f t="shared" si="2"/>
         <v>NewYork</v>
@@ -827,16 +851,20 @@
         <f t="shared" si="3"/>
         <v>8.4033613445378155</v>
       </c>
-      <c r="M19" s="2"/>
+      <c r="M19" s="2">
+        <f t="shared" si="3"/>
+        <v>6.7567567567567561</v>
+      </c>
       <c r="N19" s="2"/>
-    </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O19" s="2"/>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B20" t="str">
         <f t="shared" si="2"/>
         <v>AWS US E1</v>
       </c>
       <c r="C20" s="2">
-        <f t="shared" ref="C20:N20" si="5">100/C9</f>
+        <f t="shared" ref="C20:O20" si="5">100/C9</f>
         <v>5.2083333333333339</v>
       </c>
       <c r="D20" s="2">
@@ -854,16 +882,17 @@
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
-      <c r="M20" s="2">
+      <c r="M20" s="2"/>
+      <c r="N20" s="2">
         <f t="shared" si="5"/>
         <v>4.8780487804878048</v>
       </c>
-      <c r="N20" s="2">
+      <c r="O20" s="2">
         <f t="shared" si="5"/>
         <v>4.6511627906976747</v>
       </c>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B21" t="str">
         <f t="shared" si="2"/>
         <v>San Diego</v>
@@ -875,7 +904,7 @@
         <v>6.25</v>
       </c>
       <c r="F21" s="2">
-        <f t="shared" ref="F21:N22" si="6">100/F10</f>
+        <f t="shared" ref="F21:O22" si="6">100/F10</f>
         <v>8.4033613445378155</v>
       </c>
       <c r="G21" s="2">
@@ -903,21 +932,25 @@
         <v>9.2592592592592595</v>
       </c>
       <c r="M21" s="2">
+        <f t="shared" si="3"/>
+        <v>6.9930069930069925</v>
+      </c>
+      <c r="N21" s="2">
         <f t="shared" si="6"/>
         <v>5.3191489361702127</v>
       </c>
-      <c r="N21" s="2">
+      <c r="O21" s="2">
         <f t="shared" si="6"/>
         <v>2.2988505747126435</v>
       </c>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B22" t="str">
         <f t="shared" si="2"/>
         <v>AWS US W2</v>
       </c>
       <c r="C22" s="2">
-        <f t="shared" ref="C22:N22" si="7">100/C11</f>
+        <f t="shared" ref="C22:O22" si="7">100/C11</f>
         <v>4</v>
       </c>
       <c r="D22" s="2">
@@ -938,11 +971,12 @@
         <f t="shared" si="7"/>
         <v>13.513513513513512</v>
       </c>
-      <c r="M22" s="2">
+      <c r="M22" s="2"/>
+      <c r="N22" s="2">
         <f t="shared" si="7"/>
         <v>5</v>
       </c>
-      <c r="N22" s="2">
+      <c r="O22" s="2">
         <f t="shared" si="7"/>
         <v>4.6082949308755765</v>
       </c>

</xml_diff>